<commit_message>
delete pasta modelo que o samuel criou
</commit_message>
<xml_diff>
--- a/Plano cutover.xlsx
+++ b/Plano cutover.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f54301b22e9475d1/Documentos/Cursos/Programa Jovem Programador/Progamador de Sistemas/Projeto integrador/Projeto-integrador/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_AD4D361C20488DEA4E38A019A49B43925ADEDD94" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0816A127-C575-4A74-8120-CA20D0CE9489}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4D361C20488DEA4E38A019A49B43925ADEDD94" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{152DED78-25C3-4E4C-A19E-B20470E47DE4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,77 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Tarefa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atribuido a </t>
-  </si>
-  <si>
-    <t>Comentarios</t>
-  </si>
-  <si>
-    <t>Scene Builder:</t>
-  </si>
-  <si>
-    <t>*Criar as janelas com 3 guias</t>
-  </si>
-  <si>
-    <t>Banco de dados:</t>
-  </si>
-  <si>
-    <t>*Criar as tabelas:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>TAREFA</t>
+  </si>
+  <si>
+    <t>ATRIBUIDO A:</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>Banco de dados</t>
   </si>
   <si>
     <t>Tabela veiculo</t>
   </si>
   <si>
+    <t>Tabela marca</t>
+  </si>
+  <si>
     <t>Tabela modelo</t>
   </si>
   <si>
-    <t>Tabela marca</t>
-  </si>
-  <si>
-    <t>*Popular as banco</t>
-  </si>
-  <si>
-    <t>Aplicação java:</t>
-  </si>
-  <si>
-    <t>*Criar as classes</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>BD</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Modelos</t>
-  </si>
-  <si>
-    <t>Aplicação</t>
+    <t>Popular tabelas</t>
+  </si>
+  <si>
+    <t>Aplicação Java</t>
+  </si>
+  <si>
+    <t>Classe Controller</t>
+  </si>
+  <si>
+    <t>Classe BD</t>
+  </si>
+  <si>
+    <t>Classe modelo</t>
+  </si>
+  <si>
+    <t>Classe Service</t>
+  </si>
+  <si>
+    <t>Depependencias</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -122,9 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,106 +394,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="1" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D11" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>